<commit_message>
taskset creation and optimization algo beginning
</commit_message>
<xml_diff>
--- a/graphs/STM32F/pointer_chase/pointer_chase.xlsx
+++ b/graphs/STM32F/pointer_chase/pointer_chase.xlsx
@@ -9,7 +9,8 @@
     <sheet name="ro_FLASH-code_FLASH" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="ro_FLASH-code_CCM" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="ro_CCM-code_FLASH" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="ro_CCL-code_CCM" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="ro_CCM-code_CCM" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="ro_RAM-code_CCM" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -485,13 +486,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16201</v>
+        <v>15948</v>
       </c>
       <c r="C2" t="n">
-        <v>22171</v>
+        <v>22051</v>
       </c>
       <c r="D2" t="n">
-        <v>27773</v>
+        <v>27695</v>
       </c>
     </row>
     <row r="3">
@@ -501,13 +502,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2025</v>
+        <v>0.20262</v>
       </c>
       <c r="C3" t="n">
-        <v>0.162</v>
+        <v>0.16208</v>
       </c>
       <c r="D3" t="n">
-        <v>0.18898</v>
+        <v>0.18926</v>
       </c>
     </row>
     <row r="4">
@@ -518,17 +519,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(2361.34, 2563.84)</t>
+          <t>(4937.4, 5140.02)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(4732.64, 4894.64)</t>
+          <t>(8115.6, 8277.68)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(6800.82, 6989.8)</t>
+          <t>(10808.46, 10997.72)</t>
         </is>
       </c>
     </row>
@@ -539,13 +540,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.826</v>
+        <v>10.664</v>
       </c>
       <c r="C5" t="n">
-        <v>11.853</v>
+        <v>11.794</v>
       </c>
       <c r="D5" t="n">
-        <v>17.32</v>
+        <v>17.297</v>
       </c>
     </row>
   </sheetData>
@@ -591,13 +592,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13181</v>
+        <v>13689</v>
       </c>
       <c r="C2" t="n">
-        <v>23404</v>
+        <v>23286</v>
       </c>
       <c r="D2" t="n">
-        <v>32008</v>
+        <v>31922</v>
       </c>
     </row>
     <row r="3">
@@ -607,13 +608,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.20268</v>
+        <v>0.20258</v>
       </c>
       <c r="C3" t="n">
-        <v>0.12174</v>
+        <v>0.12178</v>
       </c>
       <c r="D3" t="n">
-        <v>0.09492</v>
+        <v>0.0948</v>
       </c>
     </row>
     <row r="4">
@@ -624,17 +625,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(2759.02, 2961.7)</t>
+          <t>(5336.42, 5539.0)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(5089.88, 5211.62)</t>
+          <t>(8474.0, 8595.78)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(7185.02, 7279.94)</t>
+          <t>(11194.08, 11288.88)</t>
         </is>
       </c>
     </row>
@@ -645,13 +646,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>8.816000000000001</v>
+        <v>9.151</v>
       </c>
       <c r="C5" t="n">
-        <v>9.401999999999999</v>
+        <v>9.358000000000001</v>
       </c>
       <c r="D5" t="n">
-        <v>10.026</v>
+        <v>9.986000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -697,13 +698,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14000</v>
+        <v>13989</v>
       </c>
       <c r="C2" t="n">
-        <v>23476</v>
+        <v>23348</v>
       </c>
       <c r="D2" t="n">
-        <v>31550</v>
+        <v>31420</v>
       </c>
     </row>
     <row r="3">
@@ -713,13 +714,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.20276</v>
+        <v>0.2027</v>
       </c>
       <c r="C3" t="n">
-        <v>0.12174</v>
+        <v>0.12186</v>
       </c>
       <c r="D3" t="n">
-        <v>0.09486</v>
+        <v>0.09497999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -730,17 +731,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(3156.92, 3359.68)</t>
+          <t>(5735.34, 5938.04)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(5406.92, 5528.66)</t>
+          <t>(8792.12, 8913.98)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(7475.14, 7570.0)</t>
+          <t>(11485.3, 11580.28)</t>
         </is>
       </c>
     </row>
@@ -751,13 +752,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>9.368</v>
+        <v>9.356999999999999</v>
       </c>
       <c r="C5" t="n">
-        <v>9.430999999999999</v>
+        <v>9.388999999999999</v>
       </c>
       <c r="D5" t="n">
-        <v>9.875999999999999</v>
+        <v>9.848000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -803,13 +804,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11407</v>
+        <v>11837</v>
       </c>
       <c r="C2" t="n">
-        <v>22891</v>
+        <v>22800</v>
       </c>
       <c r="D2" t="n">
-        <v>33848</v>
+        <v>33660</v>
       </c>
     </row>
     <row r="3">
@@ -819,13 +820,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.20246</v>
+        <v>0.20258</v>
       </c>
       <c r="C3" t="n">
-        <v>0.10142</v>
+        <v>0.1015</v>
       </c>
       <c r="D3" t="n">
-        <v>0.06782000000000001</v>
+        <v>0.0678</v>
       </c>
     </row>
     <row r="4">
@@ -836,17 +837,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(3554.86, 3757.32)</t>
+          <t>(6134.36, 6336.94)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(5723.9, 5825.32)</t>
+          <t>(9110.26, 9211.76)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(7765.2, 7833.02)</t>
+          <t>(11776.66, 11844.46)</t>
         </is>
       </c>
     </row>
@@ -857,13 +858,119 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7.621</v>
+        <v>7.913</v>
       </c>
       <c r="C5" t="n">
-        <v>7.661</v>
+        <v>7.637</v>
       </c>
       <c r="D5" t="n">
-        <v>7.575</v>
+        <v>7.531</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>intensity</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>11434</v>
+      </c>
+      <c r="C2" t="n">
+        <v>22037</v>
+      </c>
+      <c r="D2" t="n">
+        <v>32561</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>runtime</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.20258</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.10154</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.06802</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>(6932.28, 7134.86)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>(9725.94, 9827.48)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>(12331.96, 12399.98)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>energy</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>7.644</v>
+      </c>
+      <c r="C5" t="n">
+        <v>7.384</v>
+      </c>
+      <c r="D5" t="n">
+        <v>7.309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>